<commit_message>
Cambiando color en gráfica de la norma del error
</commit_message>
<xml_diff>
--- a/Concentraciones_Salida.xlsx
+++ b/Concentraciones_Salida.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,50 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>C(t = 281.250 s)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>C(t = 562.500 s)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>C(t = 843.750 s)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>C(t = 1125.000 s)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>C(t = 1406.250 s)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>C(t = 1687.500 s)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>C(t = 1968.750 s)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>C(t = 2250.000 s)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C(t = 2531.250 s)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>C(t = 2812.500 s)</t>
         </is>
@@ -492,6 +517,21 @@
       <c r="G2" t="n">
         <v>0</v>
       </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -501,18 +541,33 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
+        <v>2.232367316034164e-09</v>
+      </c>
+      <c r="D3" t="n">
         <v>1.783504813834901e-07</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
+        <v>3.450836868975576e-06</v>
+      </c>
+      <c r="F3" t="n">
         <v>2.757998277505498e-05</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
+        <v>0.0001186390809159283</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.0003328901938295575</v>
       </c>
-      <c r="F3" t="n">
+      <c r="I3" t="n">
+        <v>0.000700913902878871</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.001215663857016148</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
+        <v>0.001844089161787486</v>
+      </c>
+      <c r="L3" t="n">
         <v>0.002543563183432377</v>
       </c>
     </row>
@@ -524,18 +579,33 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
+        <v>8.416902878718349e-09</v>
+      </c>
+      <c r="D4" t="n">
         <v>6.015474148195613e-07</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>1.04860752018988e-05</v>
+      </c>
+      <c r="F4" t="n">
         <v>7.602113387504615e-05</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
+        <v>0.000301193078222778</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.0007943218949199478</v>
       </c>
-      <c r="F4" t="n">
+      <c r="I4" t="n">
+        <v>0.001599901871726558</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.002688639868058088</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
+        <v>0.003986733481069819</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.00540774982268417</v>
       </c>
     </row>
@@ -547,18 +617,33 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
+        <v>2.937991608498348e-08</v>
+      </c>
+      <c r="D5" t="n">
         <v>1.834429917316119e-06</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
+        <v>2.80407620078825e-05</v>
+      </c>
+      <c r="F5" t="n">
         <v>0.0001791297483712834</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
+        <v>0.0006365980149902988</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.001544106193731974</v>
       </c>
-      <c r="F5" t="n">
+      <c r="I5" t="n">
+        <v>0.002924585409562403</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.004698876104819573</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
+        <v>0.006740457676998732</v>
+      </c>
+      <c r="L5" t="n">
         <v>0.008918999168321212</v>
       </c>
     </row>
@@ -570,18 +655,33 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
+        <v>1.014001997939559e-07</v>
+      </c>
+      <c r="D6" t="n">
         <v>5.473568489263824e-06</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
+        <v>7.241621754445021e-05</v>
+      </c>
+      <c r="F6" t="n">
         <v>0.0004021686531089368</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
+        <v>0.001268380461844555</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.002805487525156503</v>
       </c>
-      <c r="F6" t="n">
+      <c r="I6" t="n">
+        <v>0.00495946192902</v>
+      </c>
+      <c r="J6" t="n">
         <v>0.007567893572895961</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
+        <v>0.01044186245959752</v>
+      </c>
+      <c r="L6" t="n">
         <v>0.01341205892256377</v>
       </c>
     </row>
@@ -593,18 +693,33 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
+        <v>3.476057067870299e-07</v>
+      </c>
+      <c r="D7" t="n">
         <v>1.607939412302449e-05</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
+        <v>0.0001821914338147642</v>
+      </c>
+      <c r="F7" t="n">
         <v>0.0008720868211773707</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
+        <v>0.002431980453999468</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.004897415244723817</v>
       </c>
-      <c r="F7" t="n">
+      <c r="I7" t="n">
+        <v>0.008067767955715743</v>
+      </c>
+      <c r="J7" t="n">
         <v>0.01167000960439294</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
+        <v>0.0154541337198032</v>
+      </c>
+      <c r="L7" t="n">
         <v>0.01922615366133318</v>
       </c>
     </row>
@@ -616,18 +731,33 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
+        <v>1.183245935430947e-06</v>
+      </c>
+      <c r="D8" t="n">
         <v>4.645045508293351e-05</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
+        <v>0.0004456855581129154</v>
+      </c>
+      <c r="F8" t="n">
         <v>0.001825788973116693</v>
       </c>
-      <c r="E8" t="n">
+      <c r="G8" t="n">
+        <v>0.004499813258811713</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.008262942738597109</v>
       </c>
-      <c r="F8" t="n">
+      <c r="I8" t="n">
+        <v>0.01270292747232854</v>
+      </c>
+      <c r="J8" t="n">
         <v>0.01743146468003622</v>
       </c>
-      <c r="G8" t="n">
+      <c r="K8" t="n">
+        <v>0.02215861306322456</v>
+      </c>
+      <c r="L8" t="n">
         <v>0.02669251549826675</v>
       </c>
     </row>
@@ -639,18 +769,33 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
+        <v>3.996327410193308e-06</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.000131644085833233</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
+        <v>0.001055832416525208</v>
+      </c>
+      <c r="F9" t="n">
         <v>0.003680364721890193</v>
       </c>
-      <c r="E9" t="n">
+      <c r="G9" t="n">
+        <v>0.008028289970889568</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.01348559080070524</v>
       </c>
-      <c r="F9" t="n">
+      <c r="I9" t="n">
+        <v>0.01940295517147655</v>
+      </c>
+      <c r="J9" t="n">
         <v>0.02531311660056344</v>
       </c>
-      <c r="G9" t="n">
+      <c r="K9" t="n">
+        <v>0.03093296301068205</v>
+      </c>
+      <c r="L9" t="n">
         <v>0.03611207338572522</v>
       </c>
     </row>
@@ -662,18 +807,33 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
+        <v>1.337876586823851e-05</v>
+      </c>
+      <c r="D10" t="n">
         <v>0.0003648870605121665</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
+        <v>0.002410068162060757</v>
+      </c>
+      <c r="F10" t="n">
         <v>0.007121120453368535</v>
       </c>
-      <c r="E10" t="n">
+      <c r="G10" t="n">
+        <v>0.01379268625871305</v>
+      </c>
+      <c r="H10" t="n">
         <v>0.02128148211836279</v>
       </c>
-      <c r="F10" t="n">
+      <c r="I10" t="n">
+        <v>0.02876051335476145</v>
+      </c>
+      <c r="J10" t="n">
         <v>0.03577337632609194</v>
       </c>
-      <c r="G10" t="n">
+      <c r="K10" t="n">
+        <v>0.04211502616882774</v>
+      </c>
+      <c r="L10" t="n">
         <v>0.04772364816572418</v>
       </c>
     </row>
@@ -685,18 +845,33 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
+        <v>4.43418279662544e-05</v>
+      </c>
+      <c r="D11" t="n">
         <v>0.0009851788819371572</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
+        <v>0.00526980886144969</v>
+      </c>
+      <c r="F11" t="n">
         <v>0.01318686956440259</v>
       </c>
-      <c r="E11" t="n">
+      <c r="G11" t="n">
+        <v>0.02278648389430042</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.03245305035438366</v>
       </c>
-      <c r="F11" t="n">
+      <c r="I11" t="n">
+        <v>0.04136275072255449</v>
+      </c>
+      <c r="J11" t="n">
         <v>0.04921047877710973</v>
       </c>
-      <c r="G11" t="n">
+      <c r="K11" t="n">
+        <v>0.05595381922056928</v>
+      </c>
+      <c r="L11" t="n">
         <v>0.06166491507930877</v>
       </c>
     </row>
@@ -708,18 +883,33 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
+        <v>0.0001452773225432103</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.002578511727868399</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
+        <v>0.01096958533241334</v>
+      </c>
+      <c r="F12" t="n">
         <v>0.02330819531186939</v>
       </c>
-      <c r="E12" t="n">
+      <c r="G12" t="n">
+        <v>0.03615560548679386</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.04779247156451628</v>
       </c>
-      <c r="F12" t="n">
+      <c r="I12" t="n">
+        <v>0.0576994262107754</v>
+      </c>
+      <c r="J12" t="n">
         <v>0.06588713152662223</v>
       </c>
-      <c r="G12" t="n">
+      <c r="K12" t="n">
+        <v>0.07255207155341389</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.07793046008519522</v>
       </c>
     </row>
@@ -731,18 +921,33 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
+        <v>0.000469606904874385</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.006486887781995639</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
+        <v>0.02160621834085773</v>
+      </c>
+      <c r="F13" t="n">
         <v>0.03923176245322232</v>
       </c>
-      <c r="E13" t="n">
+      <c r="G13" t="n">
+        <v>0.05504078485630945</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.06793159649777189</v>
       </c>
-      <c r="F13" t="n">
+      <c r="I13" t="n">
+        <v>0.0780452699191895</v>
+      </c>
+      <c r="J13" t="n">
         <v>0.08584566857131762</v>
       </c>
-      <c r="G13" t="n">
+      <c r="K13" t="n">
+        <v>0.09180787358880595</v>
+      </c>
+      <c r="L13" t="n">
         <v>0.09633311495490848</v>
       </c>
     </row>
@@ -754,18 +959,33 @@
         <v>0</v>
       </c>
       <c r="C14" t="n">
+        <v>0.001493946684086506</v>
+      </c>
+      <c r="D14" t="n">
         <v>0.01547307189574459</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
+        <v>0.04004942451908836</v>
+      </c>
+      <c r="F14" t="n">
         <v>0.06275963357033154</v>
       </c>
-      <c r="E14" t="n">
+      <c r="G14" t="n">
+        <v>0.08031888977300591</v>
+      </c>
+      <c r="H14" t="n">
         <v>0.0931503801427196</v>
       </c>
-      <c r="F14" t="n">
+      <c r="I14" t="n">
+        <v>0.1023320362762567</v>
+      </c>
+      <c r="J14" t="n">
         <v>0.1088270567169953</v>
       </c>
-      <c r="G14" t="n">
+      <c r="K14" t="n">
+        <v>0.1133656314305319</v>
+      </c>
+      <c r="L14" t="n">
         <v>0.1164759553453521</v>
       </c>
     </row>
@@ -777,18 +997,33 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
+        <v>0.004661597564137691</v>
+      </c>
+      <c r="D15" t="n">
         <v>0.03440630848210933</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
+        <v>0.06954706516333534</v>
+      </c>
+      <c r="F15" t="n">
         <v>0.09526788937077191</v>
       </c>
-      <c r="E15" t="n">
+      <c r="G15" t="n">
+        <v>0.1122679290953847</v>
+      </c>
+      <c r="H15" t="n">
         <v>0.1231750783658014</v>
       </c>
-      <c r="F15" t="n">
+      <c r="I15" t="n">
+        <v>0.1300349418336317</v>
+      </c>
+      <c r="J15" t="n">
         <v>0.1342109683779221</v>
       </c>
-      <c r="G15" t="n">
+      <c r="K15" t="n">
+        <v>0.1365877836199367</v>
+      </c>
+      <c r="L15" t="n">
         <v>0.1377424313087688</v>
       </c>
     </row>
@@ -800,18 +1035,33 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
+        <v>0.01419982568061658</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.07019277080179084</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
+        <v>0.1127456446648084</v>
+      </c>
+      <c r="F16" t="n">
         <v>0.1370540248471299</v>
       </c>
-      <c r="E16" t="n">
+      <c r="G16" t="n">
+        <v>0.150224198926883</v>
+      </c>
+      <c r="H16" t="n">
         <v>0.1570150835598374</v>
       </c>
-      <c r="F16" t="n">
+      <c r="I16" t="n">
+        <v>0.1601038861954337</v>
+      </c>
+      <c r="J16" t="n">
         <v>0.160995009314856</v>
       </c>
-      <c r="G16" t="n">
+      <c r="K16" t="n">
+        <v>0.1605578604796123</v>
+      </c>
+      <c r="L16" t="n">
         <v>0.1593107454938018</v>
       </c>
     </row>
@@ -823,18 +1073,33 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
+        <v>0.04423999634441782</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.1297910777735631</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
+        <v>0.1701918920722868</v>
+      </c>
+      <c r="F17" t="n">
         <v>0.1866801186695889</v>
       </c>
-      <c r="E17" t="n">
+      <c r="G17" t="n">
+        <v>0.1923376679590826</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.1928954352210764</v>
       </c>
-      <c r="F17" t="n">
+      <c r="I17" t="n">
+        <v>0.1909687527513076</v>
+      </c>
+      <c r="J17" t="n">
         <v>0.1878278171756424</v>
       </c>
-      <c r="G17" t="n">
+      <c r="K17" t="n">
+        <v>0.1841220512817366</v>
+      </c>
+      <c r="L17" t="n">
         <v>0.1801957352043832</v>
       </c>
     </row>
@@ -846,18 +1111,33 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
+        <v>0.121304769329773</v>
+      </c>
+      <c r="D18" t="n">
         <v>0.2158107641036204</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
+        <v>0.2387892194202114</v>
+      </c>
+      <c r="F18" t="n">
         <v>0.240576370053414</v>
       </c>
-      <c r="E18" t="n">
+      <c r="G18" t="n">
+        <v>0.2355421670562428</v>
+      </c>
+      <c r="H18" t="n">
         <v>0.2283337507208051</v>
       </c>
-      <c r="F18" t="n">
+      <c r="I18" t="n">
+        <v>0.220638201752436</v>
+      </c>
+      <c r="J18" t="n">
         <v>0.213102816483607</v>
       </c>
-      <c r="G18" t="n">
+      <c r="K18" t="n">
+        <v>0.2059706713562811</v>
+      </c>
+      <c r="L18" t="n">
         <v>0.1993174336630526</v>
       </c>
     </row>
@@ -869,18 +1149,33 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
+        <v>0.2720502201255362</v>
+      </c>
+      <c r="D19" t="n">
         <v>0.321250462118702</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
+        <v>0.3110339176759708</v>
+      </c>
+      <c r="F19" t="n">
         <v>0.2931770869942429</v>
       </c>
-      <c r="E19" t="n">
+      <c r="G19" t="n">
+        <v>0.2758235207359012</v>
+      </c>
+      <c r="H19" t="n">
         <v>0.2603829071026106</v>
       </c>
-      <c r="F19" t="n">
+      <c r="I19" t="n">
+        <v>0.2468932508158437</v>
+      </c>
+      <c r="J19" t="n">
         <v>0.2351079461468838</v>
       </c>
-      <c r="G19" t="n">
+      <c r="K19" t="n">
+        <v>0.2247536581809918</v>
+      </c>
+      <c r="L19" t="n">
         <v>0.2155908215039</v>
       </c>
     </row>
@@ -892,18 +1187,33 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
+        <v>0.4823758125045884</v>
+      </c>
+      <c r="D20" t="n">
         <v>0.4271727233266976</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
+        <v>0.3758281924485878</v>
+      </c>
+      <c r="F20" t="n">
         <v>0.3377314617381499</v>
       </c>
-      <c r="E20" t="n">
+      <c r="G20" t="n">
+        <v>0.3087904104941809</v>
+      </c>
+      <c r="H20" t="n">
         <v>0.2860186954358087</v>
       </c>
-      <c r="F20" t="n">
+      <c r="I20" t="n">
+        <v>0.2675541905840637</v>
+      </c>
+      <c r="J20" t="n">
         <v>0.2522140095412433</v>
       </c>
-      <c r="G20" t="n">
+      <c r="K20" t="n">
+        <v>0.2392169240534479</v>
+      </c>
+      <c r="L20" t="n">
         <v>0.2280269288785319</v>
       </c>
     </row>
@@ -915,18 +1225,33 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
+        <v>0.6790621757529187</v>
+      </c>
+      <c r="D21" t="n">
         <v>0.5069300194088409</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
+        <v>0.4210803843345883</v>
+      </c>
+      <c r="F21" t="n">
         <v>0.3676839925416395</v>
       </c>
-      <c r="E21" t="n">
+      <c r="G21" t="n">
+        <v>0.3304504322644085</v>
+      </c>
+      <c r="H21" t="n">
         <v>0.3026065231951023</v>
       </c>
-      <c r="F21" t="n">
+      <c r="I21" t="n">
+        <v>0.2807780611095</v>
+      </c>
+      <c r="J21" t="n">
         <v>0.2630736161999817</v>
       </c>
-      <c r="G21" t="n">
+      <c r="K21" t="n">
+        <v>0.2483407769128555</v>
+      </c>
+      <c r="L21" t="n">
         <v>0.2358323785802078</v>
       </c>
     </row>
@@ -938,18 +1263,33 @@
         <v>4</v>
       </c>
       <c r="C22" t="n">
+        <v>0.7598667626840945</v>
+      </c>
+      <c r="D22" t="n">
         <v>0.5367098996847754</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
+        <v>0.437354794286582</v>
+      </c>
+      <c r="F22" t="n">
         <v>0.3782526472760479</v>
       </c>
-      <c r="E22" t="n">
+      <c r="G22" t="n">
+        <v>0.3380058888268493</v>
+      </c>
+      <c r="H22" t="n">
         <v>0.3083486106778202</v>
       </c>
-      <c r="F22" t="n">
+      <c r="I22" t="n">
+        <v>0.2853307716802928</v>
+      </c>
+      <c r="J22" t="n">
         <v>0.2667971233436022</v>
       </c>
-      <c r="G22" t="n">
+      <c r="K22" t="n">
+        <v>0.2514592325607921</v>
+      </c>
+      <c r="L22" t="n">
         <v>0.2384934683411004</v>
       </c>
     </row>
@@ -961,18 +1301,33 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
+        <v>0.6790621757529187</v>
+      </c>
+      <c r="D23" t="n">
         <v>0.5069300194088409</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
+        <v>0.4210803843345883</v>
+      </c>
+      <c r="F23" t="n">
         <v>0.3676839925416394</v>
       </c>
-      <c r="E23" t="n">
+      <c r="G23" t="n">
+        <v>0.3304504322644085</v>
+      </c>
+      <c r="H23" t="n">
         <v>0.3026065231951023</v>
       </c>
-      <c r="F23" t="n">
+      <c r="I23" t="n">
+        <v>0.2807780611095</v>
+      </c>
+      <c r="J23" t="n">
         <v>0.2630736161999817</v>
       </c>
-      <c r="G23" t="n">
+      <c r="K23" t="n">
+        <v>0.2483407769128554</v>
+      </c>
+      <c r="L23" t="n">
         <v>0.2358323785802078</v>
       </c>
     </row>
@@ -984,18 +1339,33 @@
         <v>0</v>
       </c>
       <c r="C24" t="n">
+        <v>0.4823758125045884</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.4271727233266975</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
+        <v>0.3758281924485878</v>
+      </c>
+      <c r="F24" t="n">
         <v>0.3377314617381498</v>
       </c>
-      <c r="E24" t="n">
+      <c r="G24" t="n">
+        <v>0.3087904104941808</v>
+      </c>
+      <c r="H24" t="n">
         <v>0.2860186954358087</v>
       </c>
-      <c r="F24" t="n">
+      <c r="I24" t="n">
+        <v>0.2675541905840636</v>
+      </c>
+      <c r="J24" t="n">
         <v>0.2522140095412433</v>
       </c>
-      <c r="G24" t="n">
+      <c r="K24" t="n">
+        <v>0.2392169240534479</v>
+      </c>
+      <c r="L24" t="n">
         <v>0.2280269288785318</v>
       </c>
     </row>
@@ -1007,18 +1377,33 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
+        <v>0.2720502201255361</v>
+      </c>
+      <c r="D25" t="n">
         <v>0.321250462118702</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
+        <v>0.3110339176759707</v>
+      </c>
+      <c r="F25" t="n">
         <v>0.2931770869942429</v>
       </c>
-      <c r="E25" t="n">
+      <c r="G25" t="n">
+        <v>0.2758235207359012</v>
+      </c>
+      <c r="H25" t="n">
         <v>0.2603829071026105</v>
       </c>
-      <c r="F25" t="n">
+      <c r="I25" t="n">
+        <v>0.2468932508158436</v>
+      </c>
+      <c r="J25" t="n">
         <v>0.2351079461468837</v>
       </c>
-      <c r="G25" t="n">
+      <c r="K25" t="n">
+        <v>0.2247536581809917</v>
+      </c>
+      <c r="L25" t="n">
         <v>0.2155908215038999</v>
       </c>
     </row>
@@ -1030,18 +1415,33 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
+        <v>0.121304769329773</v>
+      </c>
+      <c r="D26" t="n">
         <v>0.2158107641036204</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
+        <v>0.2387892194202114</v>
+      </c>
+      <c r="F26" t="n">
         <v>0.2405763700534139</v>
       </c>
-      <c r="E26" t="n">
+      <c r="G26" t="n">
+        <v>0.2355421670562428</v>
+      </c>
+      <c r="H26" t="n">
         <v>0.228333750720805</v>
       </c>
-      <c r="F26" t="n">
+      <c r="I26" t="n">
+        <v>0.2206382017524359</v>
+      </c>
+      <c r="J26" t="n">
         <v>0.2131028164836069</v>
       </c>
-      <c r="G26" t="n">
+      <c r="K26" t="n">
+        <v>0.2059706713562809</v>
+      </c>
+      <c r="L26" t="n">
         <v>0.1993174336630525</v>
       </c>
     </row>
@@ -1053,18 +1453,33 @@
         <v>0</v>
       </c>
       <c r="C27" t="n">
+        <v>0.04423999634441782</v>
+      </c>
+      <c r="D27" t="n">
         <v>0.1297910777735631</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
+        <v>0.1701918920722867</v>
+      </c>
+      <c r="F27" t="n">
         <v>0.1866801186695889</v>
       </c>
-      <c r="E27" t="n">
+      <c r="G27" t="n">
+        <v>0.1923376679590825</v>
+      </c>
+      <c r="H27" t="n">
         <v>0.1928954352210763</v>
       </c>
-      <c r="F27" t="n">
+      <c r="I27" t="n">
+        <v>0.1909687527513075</v>
+      </c>
+      <c r="J27" t="n">
         <v>0.1878278171756423</v>
       </c>
-      <c r="G27" t="n">
+      <c r="K27" t="n">
+        <v>0.1841220512817365</v>
+      </c>
+      <c r="L27" t="n">
         <v>0.1801957352043831</v>
       </c>
     </row>
@@ -1076,18 +1491,33 @@
         <v>0</v>
       </c>
       <c r="C28" t="n">
+        <v>0.01419982568061658</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.07019277080179083</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
+        <v>0.1127456446648083</v>
+      </c>
+      <c r="F28" t="n">
         <v>0.1370540248471299</v>
       </c>
-      <c r="E28" t="n">
+      <c r="G28" t="n">
+        <v>0.1502241989268829</v>
+      </c>
+      <c r="H28" t="n">
         <v>0.1570150835598373</v>
       </c>
-      <c r="F28" t="n">
+      <c r="I28" t="n">
+        <v>0.1601038861954336</v>
+      </c>
+      <c r="J28" t="n">
         <v>0.1609950093148559</v>
       </c>
-      <c r="G28" t="n">
+      <c r="K28" t="n">
+        <v>0.1605578604796122</v>
+      </c>
+      <c r="L28" t="n">
         <v>0.1593107454938017</v>
       </c>
     </row>
@@ -1099,18 +1529,33 @@
         <v>0</v>
       </c>
       <c r="C29" t="n">
+        <v>0.004661597564137689</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.03440630848210931</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
+        <v>0.06954706516333531</v>
+      </c>
+      <c r="F29" t="n">
         <v>0.09526788937077188</v>
       </c>
-      <c r="E29" t="n">
+      <c r="G29" t="n">
+        <v>0.1122679290953846</v>
+      </c>
+      <c r="H29" t="n">
         <v>0.1231750783658013</v>
       </c>
-      <c r="F29" t="n">
+      <c r="I29" t="n">
+        <v>0.1300349418336316</v>
+      </c>
+      <c r="J29" t="n">
         <v>0.134210968377922</v>
       </c>
-      <c r="G29" t="n">
+      <c r="K29" t="n">
+        <v>0.1365877836199366</v>
+      </c>
+      <c r="L29" t="n">
         <v>0.1377424313087687</v>
       </c>
     </row>
@@ -1122,18 +1567,33 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
+        <v>0.001493946684086505</v>
+      </c>
+      <c r="D30" t="n">
         <v>0.01547307189574458</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
+        <v>0.04004942451908834</v>
+      </c>
+      <c r="F30" t="n">
         <v>0.06275963357033153</v>
       </c>
-      <c r="E30" t="n">
+      <c r="G30" t="n">
+        <v>0.08031888977300586</v>
+      </c>
+      <c r="H30" t="n">
         <v>0.09315038014271954</v>
       </c>
-      <c r="F30" t="n">
+      <c r="I30" t="n">
+        <v>0.1023320362762566</v>
+      </c>
+      <c r="J30" t="n">
         <v>0.1088270567169952</v>
       </c>
-      <c r="G30" t="n">
+      <c r="K30" t="n">
+        <v>0.1133656314305318</v>
+      </c>
+      <c r="L30" t="n">
         <v>0.116475955345352</v>
       </c>
     </row>
@@ -1145,18 +1605,33 @@
         <v>0</v>
       </c>
       <c r="C31" t="n">
+        <v>0.0004696069048743845</v>
+      </c>
+      <c r="D31" t="n">
         <v>0.006486887781995635</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
+        <v>0.02160621834085771</v>
+      </c>
+      <c r="F31" t="n">
         <v>0.0392317624532223</v>
       </c>
-      <c r="E31" t="n">
+      <c r="G31" t="n">
+        <v>0.05504078485630941</v>
+      </c>
+      <c r="H31" t="n">
         <v>0.06793159649777183</v>
       </c>
-      <c r="F31" t="n">
+      <c r="I31" t="n">
+        <v>0.07804526991918945</v>
+      </c>
+      <c r="J31" t="n">
         <v>0.08584566857131753</v>
       </c>
-      <c r="G31" t="n">
+      <c r="K31" t="n">
+        <v>0.09180787358880582</v>
+      </c>
+      <c r="L31" t="n">
         <v>0.09633311495490837</v>
       </c>
     </row>
@@ -1168,18 +1643,33 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
+        <v>0.0001452773225432102</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.002578511727868397</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
+        <v>0.01096958533241334</v>
+      </c>
+      <c r="F32" t="n">
         <v>0.02330819531186937</v>
       </c>
-      <c r="E32" t="n">
+      <c r="G32" t="n">
+        <v>0.03615560548679383</v>
+      </c>
+      <c r="H32" t="n">
         <v>0.04779247156451623</v>
       </c>
-      <c r="F32" t="n">
+      <c r="I32" t="n">
+        <v>0.05769942621077533</v>
+      </c>
+      <c r="J32" t="n">
         <v>0.06588713152662216</v>
       </c>
-      <c r="G32" t="n">
+      <c r="K32" t="n">
+        <v>0.07255207155341381</v>
+      </c>
+      <c r="L32" t="n">
         <v>0.07793046008519512</v>
       </c>
     </row>
@@ -1191,18 +1681,33 @@
         <v>0</v>
       </c>
       <c r="C33" t="n">
+        <v>4.434182796625434e-05</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.0009851788819371563</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
+        <v>0.005269808861449685</v>
+      </c>
+      <c r="F33" t="n">
         <v>0.01318686956440258</v>
       </c>
-      <c r="E33" t="n">
+      <c r="G33" t="n">
+        <v>0.0227864838943004</v>
+      </c>
+      <c r="H33" t="n">
         <v>0.03245305035438363</v>
       </c>
-      <c r="F33" t="n">
+      <c r="I33" t="n">
+        <v>0.04136275072255445</v>
+      </c>
+      <c r="J33" t="n">
         <v>0.04921047877710967</v>
       </c>
-      <c r="G33" t="n">
+      <c r="K33" t="n">
+        <v>0.05595381922056921</v>
+      </c>
+      <c r="L33" t="n">
         <v>0.06166491507930867</v>
       </c>
     </row>
@@ -1214,18 +1719,33 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
+        <v>1.337876586823849e-05</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.0003648870605121661</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
+        <v>0.002410068162060754</v>
+      </c>
+      <c r="F34" t="n">
         <v>0.007121120453368528</v>
       </c>
-      <c r="E34" t="n">
+      <c r="G34" t="n">
+        <v>0.01379268625871304</v>
+      </c>
+      <c r="H34" t="n">
         <v>0.02128148211836277</v>
       </c>
-      <c r="F34" t="n">
+      <c r="I34" t="n">
+        <v>0.02876051335476142</v>
+      </c>
+      <c r="J34" t="n">
         <v>0.03577337632609189</v>
       </c>
-      <c r="G34" t="n">
+      <c r="K34" t="n">
+        <v>0.04211502616882767</v>
+      </c>
+      <c r="L34" t="n">
         <v>0.04772364816572411</v>
       </c>
     </row>
@@ -1237,18 +1757,33 @@
         <v>0</v>
       </c>
       <c r="C35" t="n">
+        <v>3.996327410193301e-06</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.0001316440858332329</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
+        <v>0.001055832416525207</v>
+      </c>
+      <c r="F35" t="n">
         <v>0.003680364721890188</v>
       </c>
-      <c r="E35" t="n">
+      <c r="G35" t="n">
+        <v>0.008028289970889561</v>
+      </c>
+      <c r="H35" t="n">
         <v>0.01348559080070522</v>
       </c>
-      <c r="F35" t="n">
+      <c r="I35" t="n">
+        <v>0.01940295517147653</v>
+      </c>
+      <c r="J35" t="n">
         <v>0.02531311660056341</v>
       </c>
-      <c r="G35" t="n">
+      <c r="K35" t="n">
+        <v>0.03093296301068201</v>
+      </c>
+      <c r="L35" t="n">
         <v>0.03611207338572516</v>
       </c>
     </row>
@@ -1260,18 +1795,33 @@
         <v>0</v>
       </c>
       <c r="C36" t="n">
+        <v>1.183245935430945e-06</v>
+      </c>
+      <c r="D36" t="n">
         <v>4.645045508293343e-05</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
+        <v>0.0004456855581129147</v>
+      </c>
+      <c r="F36" t="n">
         <v>0.001825788973116691</v>
       </c>
-      <c r="E36" t="n">
+      <c r="G36" t="n">
+        <v>0.004499813258811708</v>
+      </c>
+      <c r="H36" t="n">
         <v>0.008262942738597099</v>
       </c>
-      <c r="F36" t="n">
+      <c r="I36" t="n">
+        <v>0.01270292747232853</v>
+      </c>
+      <c r="J36" t="n">
         <v>0.0174314646800362</v>
       </c>
-      <c r="G36" t="n">
+      <c r="K36" t="n">
+        <v>0.02215861306322452</v>
+      </c>
+      <c r="L36" t="n">
         <v>0.02669251549826671</v>
       </c>
     </row>
@@ -1283,18 +1833,33 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
+        <v>3.476057067870293e-07</v>
+      </c>
+      <c r="D37" t="n">
         <v>1.607939412302446e-05</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
+        <v>0.000182191433814764</v>
+      </c>
+      <c r="F37" t="n">
         <v>0.0008720868211773696</v>
       </c>
-      <c r="E37" t="n">
+      <c r="G37" t="n">
+        <v>0.002431980453999465</v>
+      </c>
+      <c r="H37" t="n">
         <v>0.00489741524472381</v>
       </c>
-      <c r="F37" t="n">
+      <c r="I37" t="n">
+        <v>0.008067767955715731</v>
+      </c>
+      <c r="J37" t="n">
         <v>0.01167000960439292</v>
       </c>
-      <c r="G37" t="n">
+      <c r="K37" t="n">
+        <v>0.01545413371980317</v>
+      </c>
+      <c r="L37" t="n">
         <v>0.01922615366133314</v>
       </c>
     </row>
@@ -1306,18 +1871,33 @@
         <v>0</v>
       </c>
       <c r="C38" t="n">
+        <v>1.014001997939557e-07</v>
+      </c>
+      <c r="D38" t="n">
         <v>5.473568489263814e-06</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
+        <v>7.24162175444501e-05</v>
+      </c>
+      <c r="F38" t="n">
         <v>0.0004021686531089362</v>
       </c>
-      <c r="E38" t="n">
+      <c r="G38" t="n">
+        <v>0.001268380461844554</v>
+      </c>
+      <c r="H38" t="n">
         <v>0.0028054875251565</v>
       </c>
-      <c r="F38" t="n">
+      <c r="I38" t="n">
+        <v>0.004959461929019994</v>
+      </c>
+      <c r="J38" t="n">
         <v>0.00756789357289595</v>
       </c>
-      <c r="G38" t="n">
+      <c r="K38" t="n">
+        <v>0.0104418624595975</v>
+      </c>
+      <c r="L38" t="n">
         <v>0.01341205892256375</v>
       </c>
     </row>
@@ -1329,18 +1909,33 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
+        <v>2.937991608498342e-08</v>
+      </c>
+      <c r="D39" t="n">
         <v>1.834429917316115e-06</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
+        <v>2.804076200788245e-05</v>
+      </c>
+      <c r="F39" t="n">
         <v>0.0001791297483712831</v>
       </c>
-      <c r="E39" t="n">
+      <c r="G39" t="n">
+        <v>0.0006365980149902978</v>
+      </c>
+      <c r="H39" t="n">
         <v>0.001544106193731972</v>
       </c>
-      <c r="F39" t="n">
+      <c r="I39" t="n">
+        <v>0.002924585409562398</v>
+      </c>
+      <c r="J39" t="n">
         <v>0.004698876104819566</v>
       </c>
-      <c r="G39" t="n">
+      <c r="K39" t="n">
+        <v>0.00674045767699872</v>
+      </c>
+      <c r="L39" t="n">
         <v>0.008918999168321194</v>
       </c>
     </row>
@@ -1352,18 +1947,33 @@
         <v>0</v>
       </c>
       <c r="C40" t="n">
+        <v>8.416902878718331e-09</v>
+      </c>
+      <c r="D40" t="n">
         <v>6.0154741481956e-07</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
+        <v>1.048607520189878e-05</v>
+      </c>
+      <c r="F40" t="n">
         <v>7.602113387504601e-05</v>
       </c>
-      <c r="E40" t="n">
+      <c r="G40" t="n">
+        <v>0.0003011930782227775</v>
+      </c>
+      <c r="H40" t="n">
         <v>0.0007943218949199465</v>
       </c>
-      <c r="F40" t="n">
+      <c r="I40" t="n">
+        <v>0.001599901871726555</v>
+      </c>
+      <c r="J40" t="n">
         <v>0.002688639868058083</v>
       </c>
-      <c r="G40" t="n">
+      <c r="K40" t="n">
+        <v>0.003986733481069812</v>
+      </c>
+      <c r="L40" t="n">
         <v>0.005407749822684159</v>
       </c>
     </row>
@@ -1375,18 +1985,33 @@
         <v>0</v>
       </c>
       <c r="C41" t="n">
+        <v>2.232367316034159e-09</v>
+      </c>
+      <c r="D41" t="n">
         <v>1.783504813834897e-07</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
+        <v>3.450836868975569e-06</v>
+      </c>
+      <c r="F41" t="n">
         <v>2.757998277505493e-05</v>
       </c>
-      <c r="E41" t="n">
+      <c r="G41" t="n">
+        <v>0.0001186390809159281</v>
+      </c>
+      <c r="H41" t="n">
         <v>0.0003328901938295569</v>
       </c>
-      <c r="F41" t="n">
+      <c r="I41" t="n">
+        <v>0.0007009139028788698</v>
+      </c>
+      <c r="J41" t="n">
         <v>0.001215663857016146</v>
       </c>
-      <c r="G41" t="n">
+      <c r="K41" t="n">
+        <v>0.001844089161787483</v>
+      </c>
+      <c r="L41" t="n">
         <v>0.002543563183432372</v>
       </c>
     </row>
@@ -1410,6 +2035,21 @@
         <v>0</v>
       </c>
       <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
+      <c r="L42" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>